<commit_message>
designed holder and fixed up files
</commit_message>
<xml_diff>
--- a/template_dimensions.xlsx
+++ b/template_dimensions.xlsx
@@ -4,17 +4,52 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="84" windowWidth="10392" windowHeight="5856"/>
+    <workbookView xWindow="192" yWindow="84" windowWidth="10392" windowHeight="5856" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="dimensions" sheetId="1" r:id="rId1"/>
+    <sheet name="templates" sheetId="1" r:id="rId1"/>
+    <sheet name="holder" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Daniel Smith</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Daniel Smith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+outer chord length for curves</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="65">
   <si>
     <t>Template</t>
   </si>
@@ -131,13 +166,91 @@
   </si>
   <si>
     <t>Final measurements</t>
+  </si>
+  <si>
+    <t>Not all layers will have all templates - lower layers will have solid parts to hold up shorter templates</t>
+  </si>
+  <si>
+    <t>The bottom will, of course, be fully solid</t>
+  </si>
+  <si>
+    <t>The lid will be built similarly.</t>
+  </si>
+  <si>
+    <t>Figure 1 to the right describes rough template locations</t>
+  </si>
+  <si>
+    <t>2s</t>
+  </si>
+  <si>
+    <t>1s (vertical)</t>
+  </si>
+  <si>
+    <t>3s</t>
+  </si>
+  <si>
+    <t>4s</t>
+  </si>
+  <si>
+    <t>5s</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Template Length</t>
+  </si>
+  <si>
+    <t>Slot Length</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>Slot Width</t>
+  </si>
+  <si>
+    <t>All gaps should be &gt;=3mm</t>
+  </si>
+  <si>
+    <t>Swap the 5s to the innermost row</t>
+  </si>
+  <si>
+    <t>widest row</t>
+  </si>
+  <si>
+    <t>Base length</t>
+  </si>
+  <si>
+    <t>Base Width</t>
+  </si>
+  <si>
+    <t>Top layer (all cuts)</t>
+  </si>
+  <si>
+    <t>Bottom layer (no cuts)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +275,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +302,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -185,16 +317,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -207,6 +429,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>404914</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5600700" y="0"/>
+          <a:ext cx="12162574" cy="4671465"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,4 +1554,793 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="2.109375" customWidth="1"/>
+    <col min="14" max="14" width="6.109375" customWidth="1"/>
+    <col min="16" max="16" width="6.109375" customWidth="1"/>
+    <col min="17" max="17" width="6.77734375" customWidth="1"/>
+    <col min="18" max="18" width="2.21875" customWidth="1"/>
+    <col min="19" max="19" width="3.109375" customWidth="1"/>
+    <col min="21" max="21" width="2.21875" customWidth="1"/>
+    <col min="23" max="23" width="2.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <f>B9+3</f>
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C19" si="0">B10+3</f>
+        <v>83</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2">
+        <v>120</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2">
+        <v>160</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>163</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2">
+        <v>200</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>203</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>70.647999999999996</v>
+      </c>
+      <c r="C14">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>108.48800000000001</v>
+      </c>
+      <c r="C15">
+        <v>112</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>146.37600000000003</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>64.275999999999996</v>
+      </c>
+      <c r="C17">
+        <v>68</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18">
+        <v>102.196</v>
+      </c>
+      <c r="C18">
+        <v>106</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>140.34800000000001</v>
+      </c>
+      <c r="C19">
+        <v>144</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <f>7*3+6*4</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24">
+        <f>E36</f>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="7"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <f>SUM(J30:W30)</f>
+        <v>209</v>
+      </c>
+      <c r="J30" s="8">
+        <v>3</v>
+      </c>
+      <c r="K30" s="14">
+        <f>C13</f>
+        <v>203</v>
+      </c>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="8"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="10"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <f>SUM(J32:W32)</f>
+        <v>215</v>
+      </c>
+      <c r="J32" s="8">
+        <v>3</v>
+      </c>
+      <c r="K32" s="14">
+        <f>C12</f>
+        <v>163</v>
+      </c>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="14">
+        <f>C9</f>
+        <v>23</v>
+      </c>
+      <c r="U32" s="9"/>
+      <c r="V32" s="14">
+        <f>T32</f>
+        <v>23</v>
+      </c>
+      <c r="W32" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="8"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="10"/>
+    </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <f>SUM(J34:W34)</f>
+        <v>212</v>
+      </c>
+      <c r="J34" s="8">
+        <v>3</v>
+      </c>
+      <c r="K34" s="14">
+        <f>C11</f>
+        <v>123</v>
+      </c>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14">
+        <f>C10</f>
+        <v>83</v>
+      </c>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="8"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="10"/>
+    </row>
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36">
+        <f>SUM(J36:W36)</f>
+        <v>228</v>
+      </c>
+      <c r="J36" s="8">
+        <v>3</v>
+      </c>
+      <c r="K36" s="14">
+        <f>C16</f>
+        <v>150</v>
+      </c>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="9">
+        <v>4</v>
+      </c>
+      <c r="S36" s="14">
+        <f>C17</f>
+        <v>68</v>
+      </c>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="8"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
+      <c r="W37" s="10"/>
+    </row>
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <f>SUM(J38:W38)</f>
+        <v>224</v>
+      </c>
+      <c r="J38" s="8">
+        <v>3</v>
+      </c>
+      <c r="K38" s="14">
+        <f>C15</f>
+        <v>112</v>
+      </c>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="14">
+        <f>C18</f>
+        <v>106</v>
+      </c>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J39" s="8"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="10"/>
+    </row>
+    <row r="40" spans="2:23" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <f>SUM(J40:W40)</f>
+        <v>224</v>
+      </c>
+      <c r="J40" s="8">
+        <v>3</v>
+      </c>
+      <c r="K40" s="14">
+        <f>C14</f>
+        <v>74</v>
+      </c>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="14">
+        <f>C19</f>
+        <v>144</v>
+      </c>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J41" s="11"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12"/>
+      <c r="S41" s="12"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="13"/>
+    </row>
+    <row r="43" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="J44" s="5"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+      <c r="U44" s="6"/>
+      <c r="V44" s="6"/>
+      <c r="W44" s="7"/>
+    </row>
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="J45" s="8"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="9"/>
+      <c r="U45" s="9"/>
+      <c r="V45" s="9"/>
+      <c r="W45" s="10"/>
+    </row>
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <f>228-203</f>
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <f>B46/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="J46" s="8"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="W46" s="10"/>
+    </row>
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="J47" s="8"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="10"/>
+    </row>
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="J48" s="8"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="10"/>
+    </row>
+    <row r="49" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f>228-163-3-3-23-23</f>
+        <v>13</v>
+      </c>
+      <c r="J49" s="8"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9">
+        <f>B24</f>
+        <v>228</v>
+      </c>
+      <c r="P49" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q49" s="9">
+        <f>B23</f>
+        <v>45</v>
+      </c>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+      <c r="V49" s="9"/>
+      <c r="W49" s="10"/>
+    </row>
+    <row r="50" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f>C49/2</f>
+        <v>6.5</v>
+      </c>
+      <c r="J50" s="8"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="10"/>
+    </row>
+    <row r="51" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="J51" s="8"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="10"/>
+    </row>
+    <row r="52" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="J52" s="8"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="9"/>
+      <c r="S52" s="9"/>
+      <c r="T52" s="9"/>
+      <c r="U52" s="9"/>
+      <c r="V52" s="9"/>
+      <c r="W52" s="10"/>
+    </row>
+    <row r="53" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="J53" s="8"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="9"/>
+      <c r="V53" s="9"/>
+      <c r="W53" s="10"/>
+    </row>
+    <row r="54" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="J54" s="8"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="10"/>
+    </row>
+    <row r="55" spans="3:23" x14ac:dyDescent="0.3">
+      <c r="J55" s="8"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="10"/>
+    </row>
+    <row r="56" spans="3:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J56" s="11"/>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="12"/>
+      <c r="U56" s="12"/>
+      <c r="V56" s="12"/>
+      <c r="W56" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>